<commit_message>
UT has beeen added
</commit_message>
<xml_diff>
--- a/SpearHead.Tests/TestData/Sample Excel_valid.xlsx
+++ b/SpearHead.Tests/TestData/Sample Excel_valid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\.Net Projects\Upwork\SpearHead\SpearHead.Tests\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAF7B90C-E0A4-44E1-9AFF-2594DB9BB5DA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB4DC474-1806-44CC-8A86-488D9452C94E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{8A231B14-E53F-4DA4-9F7E-B09CC06CECC2}"/>
   </bookViews>
@@ -32,26 +32,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="12">
   <si>
     <t>Packet</t>
   </si>
   <si>
-    <t>Product</t>
-  </si>
-  <si>
-    <t>wt</t>
-  </si>
-  <si>
-    <t>color</t>
-  </si>
-  <si>
     <t>prod1</t>
   </si>
   <si>
-    <t>red</t>
-  </si>
-  <si>
     <t>PacketId</t>
   </si>
   <si>
@@ -73,10 +61,13 @@
     <t>P3</t>
   </si>
   <si>
-    <t>Pd1</t>
-  </si>
-  <si>
-    <t>Pd2</t>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Sallary</t>
   </si>
 </sst>
 </file>
@@ -112,8 +103,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -428,58 +420,72 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1D7CABA-30B9-4828-83FE-AFB9CF0454BF}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B2" s="1">
+        <v>20</v>
+      </c>
+      <c r="C2">
+        <v>60000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>14</v>
+      <c r="B3" s="1">
+        <v>20</v>
       </c>
       <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>22</v>
+      </c>
+      <c r="C4">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>23</v>
+      </c>
+      <c r="C5">
+        <v>60000</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -495,7 +501,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -503,26 +509,26 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
         <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -542,7 +548,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -550,26 +556,26 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>